<commit_message>
ajustes pedidos crud y vista tabla (fronted)
</commit_message>
<xml_diff>
--- a/planning/assets/formatsXlsx/Inventario.xlsx
+++ b/planning/assets/formatsXlsx/Inventario.xlsx
@@ -13,35 +13,53 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Autor</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Si es un producto deje el campo vacio</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>referencia_producto</t>
-  </si>
-  <si>
-    <t>producto</t>
-  </si>
-  <si>
-    <t>cantidad_producto</t>
-  </si>
-  <si>
-    <t>referencia_material</t>
-  </si>
-  <si>
-    <t>material</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>unidad</t>
   </si>
   <si>
-    <t>cantidad_material</t>
+    <t>referencia</t>
+  </si>
+  <si>
+    <t>nombre</t>
+  </si>
+  <si>
+    <t>cantidad</t>
+  </si>
+  <si>
+    <t>categoria</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +92,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -99,7 +124,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -108,10 +133,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -119,7 +147,7 @@
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="7">
     <dxf>
       <font>
         <strike val="0"/>
@@ -132,7 +160,6 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -147,7 +174,6 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -162,7 +188,6 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -177,7 +202,6 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -192,7 +216,6 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -207,37 +230,6 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -252,7 +244,6 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -261,15 +252,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="A1:G6" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <tableColumns count="7">
-    <tableColumn id="1" name="referencia_producto" dataDxfId="6"/>
-    <tableColumn id="2" name="producto" dataDxfId="5"/>
-    <tableColumn id="3" name="cantidad_producto" dataDxfId="4"/>
-    <tableColumn id="4" name="referencia_material" dataDxfId="3"/>
-    <tableColumn id="5" name="material" dataDxfId="2"/>
-    <tableColumn id="6" name="unidad" dataDxfId="1"/>
-    <tableColumn id="7" name="cantidad_material" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:E7" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <tableColumns count="5">
+    <tableColumn id="1" name="referencia" dataDxfId="4"/>
+    <tableColumn id="2" name="nombre" dataDxfId="3"/>
+    <tableColumn id="3" name="unidad" dataDxfId="2"/>
+    <tableColumn id="4" name="cantidad" dataDxfId="1"/>
+    <tableColumn id="5" name="categoria" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -560,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -588,15 +577,15 @@
     <col min="18" max="18" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18">
+    <row r="1" spans="1:5" ht="18">
       <c r="A1" s="5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>3</v>
@@ -604,57 +593,84 @@
       <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:7">
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7">
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7">
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7">
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="16" spans="1:5" ht="21">
+      <c r="D16" s="2"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="4:6" ht="21">
+      <c r="D17" s="2"/>
+      <c r="E17" s="3"/>
     </row>
     <row r="18" spans="4:6" ht="21">
       <c r="D18" s="2"/>
@@ -695,24 +711,24 @@
       <c r="E25" s="3"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="4:6" ht="21">
-      <c r="D26" s="2"/>
-      <c r="E26" s="3"/>
+    <row r="26" spans="4:6">
+      <c r="D26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="4:6" ht="21">
-      <c r="D27" s="2"/>
-      <c r="E27" s="3"/>
+    <row r="27" spans="4:6">
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="4:6">
-      <c r="D28" s="1"/>
-    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7">
+      <formula1>"Productos,Materiales,Insumos"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Separacion accesos de usuario (costos y planeacion)
</commit_message>
<xml_diff>
--- a/planning/assets/formatsXlsx/Inventario.xlsx
+++ b/planning/assets/formatsXlsx/Inventario.xlsx
@@ -27,6 +27,34 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Si la categoria no es producto, dejar los dos campos de moldes vacios</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Si la categoria no es producto, dejar los dos campos de moldes vacios</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t>Si es un producto deje el campo vacio</t>
@@ -38,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>unidad</t>
   </si>
@@ -54,12 +82,18 @@
   <si>
     <t>categoria</t>
   </si>
+  <si>
+    <t>referencia_molde</t>
+  </si>
+  <si>
+    <t>molde</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,6 +133,23 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -124,7 +175,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -142,15 +193,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="9">
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -164,7 +225,11 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -174,7 +239,43 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -252,13 +353,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:E7" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <tableColumns count="5">
-    <tableColumn id="1" name="referencia" dataDxfId="4"/>
-    <tableColumn id="2" name="nombre" dataDxfId="3"/>
-    <tableColumn id="3" name="unidad" dataDxfId="2"/>
-    <tableColumn id="4" name="cantidad" dataDxfId="1"/>
-    <tableColumn id="5" name="categoria" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:G7" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <tableColumns count="7">
+    <tableColumn id="1" name="referencia" dataDxfId="6"/>
+    <tableColumn id="2" name="nombre" dataDxfId="5"/>
+    <tableColumn id="3" name="referencia_molde" dataDxfId="4"/>
+    <tableColumn id="4" name="molde" dataDxfId="3"/>
+    <tableColumn id="5" name="unidad" dataDxfId="2"/>
+    <tableColumn id="6" name="cantidad" dataDxfId="1"/>
+    <tableColumn id="7" name="categoria" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -549,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -562,7 +665,7 @@
     <col min="3" max="3" width="35.28515625" customWidth="1"/>
     <col min="4" max="4" width="34.5703125" customWidth="1"/>
     <col min="5" max="5" width="23.140625" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
     <col min="7" max="7" width="32.5703125" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" customWidth="1"/>
     <col min="9" max="9" width="15.42578125" customWidth="1"/>
@@ -577,94 +680,112 @@
     <col min="18" max="18" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18">
+    <row r="1" spans="1:7" ht="18">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:7">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:7">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:7">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="16" spans="1:5" ht="21">
+    <row r="16" spans="1:7" ht="21">
       <c r="D16" s="2"/>
       <c r="E16" s="3"/>
     </row>
@@ -720,7 +841,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G7">
       <formula1>"Productos,Materiales,Insumos"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>